<commit_message>
Adding the first two parts of Weather Data Collector Scheduler with Ftpscheduler and Meteoblue API Call
</commit_message>
<xml_diff>
--- a/InventarStatischeSensoren.xlsx
+++ b/InventarStatischeSensoren.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a033289c0c47cfbd/Desktop/Vaishnavi/Web and Data Science/Research_Assistant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{D61D7F6A-73D9-42B7-965C-1DC022110C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43DCCCBA-143A-4594-BE7D-C2E9F60F5791}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E2F20691-EECB-41AA-91B0-7B6549BEF2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{062A77DD-C5E7-4C2C-9ABF-1BCC8D38E35A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="100">
   <si>
     <t>SN</t>
   </si>
@@ -314,25 +314,39 @@
     <t>Weatherstation</t>
   </si>
   <si>
+    <t>Bremm Kirchbach (WS)</t>
+  </si>
+  <si>
     <t>Arena Unten</t>
   </si>
   <si>
     <t>Arena Oben</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,8 +359,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -354,14 +374,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +632,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +696,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -740,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -827,305 +867,308 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>108</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>181</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6">
+        <v>198</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>210</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4">
+        <v>240</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4">
+        <v>180</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4">
+        <v>193</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4">
+        <v>150</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4">
+        <v>178</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4">
+        <v>221</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="4">
+        <v>243</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="4">
+        <v>96</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="6">
+        <v>182</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="4">
+        <v>181</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>198</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>210</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>240</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7">
-        <v>180</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <v>193</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9">
-        <v>150</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10">
-        <v>178</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11">
-        <v>221</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12">
-        <v>243</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13">
-        <v>96</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14">
-        <v>182</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15">
-        <v>181</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>119</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>196</v>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
+      <c r="D17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1134,7 +1177,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,23 +1243,23 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1331,22 +1374,23 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">

</xml_diff>